<commit_message>
Add TaiShiCi Quest Animations
</commit_message>
<xml_diff>
--- a/Excels/SchemaItems.xlsx
+++ b/Excels/SchemaItems.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\潘鹏\Documents\Codes\Games\TKS-R\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\潘鹏\Documents\GitHub\TKSR\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757AB7AA-1601-4A11-A1E9-14DC80988C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4F8314-6AA4-42CF-9F3A-BAFEE3C8AF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1614" uniqueCount="884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="888">
   <si>
     <t>Id</t>
   </si>
@@ -3204,6 +3204,22 @@
   </si>
   <si>
     <t>QuestPropCnt_YingXiongZui</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestPropCnt_ChouMaZhiHua</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestPropCnt_ManTuoLuoGuo</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>臭麻子花</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>曼陀罗果</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -3749,8 +3765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2BF42B-B9E6-4AA7-A0C5-A2602055F321}">
   <dimension ref="A1:H500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="H305" sqref="H305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.25" x14ac:dyDescent="0.15"/>
@@ -11065,7 +11081,7 @@
         <v>8042</v>
       </c>
       <c r="B304" s="14" t="s">
-        <v>761</v>
+        <v>886</v>
       </c>
       <c r="C304" s="14">
         <v>0</v>
@@ -11082,14 +11098,16 @@
       <c r="G304" s="14">
         <v>6</v>
       </c>
-      <c r="H304" s="14"/>
+      <c r="H304" s="14" t="s">
+        <v>884</v>
+      </c>
     </row>
     <row r="305" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A305" s="14">
         <v>8043</v>
       </c>
       <c r="B305" s="14" t="s">
-        <v>763</v>
+        <v>887</v>
       </c>
       <c r="C305" s="14">
         <v>0</v>
@@ -11106,7 +11124,9 @@
       <c r="G305" s="14">
         <v>6</v>
       </c>
-      <c r="H305" s="14"/>
+      <c r="H305" s="14" t="s">
+        <v>885</v>
+      </c>
     </row>
     <row r="306" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A306" s="14">
@@ -20469,8 +20489,8 @@
   <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.25" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Update Tiger Meat Quest
</commit_message>
<xml_diff>
--- a/Excels/SchemaItems.xlsx
+++ b/Excels/SchemaItems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\GitHub\TKSR\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EBC313-361D-4854-BF35-437CBA7B2717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC79BDC-1876-4C5A-8654-89A572DE97D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="909">
   <si>
     <t>Id</t>
   </si>
@@ -3300,6 +3300,10 @@
   </si>
   <si>
     <t>董卓军军服</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestPropCnt_HuRou</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -3827,8 +3831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2BF42B-B9E6-4AA7-A0C5-A2602055F321}">
   <dimension ref="A1:H337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
-      <selection activeCell="H299" sqref="H299"/>
+    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
+      <selection activeCell="H318" sqref="H318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -11522,7 +11526,9 @@
       <c r="G318" s="10">
         <v>6</v>
       </c>
-      <c r="H318" s="10"/>
+      <c r="H318" s="10" t="s">
+        <v>908</v>
+      </c>
     </row>
     <row r="319" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A319" s="10">

</xml_diff>

<commit_message>
Finished HuaShan ManTuoLuoGuo Task
</commit_message>
<xml_diff>
--- a/Excels/SchemaItems.xlsx
+++ b/Excels/SchemaItems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\GitHub\TKSR\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC79BDC-1876-4C5A-8654-89A572DE97D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17C5874-6E35-4F96-B3ED-7CB59846A31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="909">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="908">
   <si>
     <t>Id</t>
   </si>
@@ -2772,9 +2772,6 @@
   </si>
   <si>
     <t>Topaz-Mu_44-1</t>
-  </si>
-  <si>
-    <t>曼陀罗果</t>
   </si>
   <si>
     <t>Topaz-Mu_35-1</t>
@@ -3831,8 +3828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2BF42B-B9E6-4AA7-A0C5-A2602055F321}">
   <dimension ref="A1:H337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
-      <selection activeCell="H318" sqref="H318"/>
+    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="H305" sqref="H305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -3869,7 +3866,7 @@
         <v>57</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -3921,7 +3918,7 @@
         <v>56</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3947,7 +3944,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3973,7 +3970,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3999,7 +3996,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4649,7 +4646,7 @@
         <v>2</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4681,7 +4678,7 @@
         <v>8004</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C35" s="4">
         <v>2</v>
@@ -4699,7 +4696,7 @@
         <v>2</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5067,7 +5064,7 @@
         <v>207</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C51" s="4">
         <v>2</v>
@@ -5085,7 +5082,7 @@
         <v>2</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5141,7 +5138,7 @@
         <v>210</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C54" s="4">
         <v>2</v>
@@ -5159,7 +5156,7 @@
         <v>2</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5215,7 +5212,7 @@
         <v>213</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="C57" s="4">
         <v>2</v>
@@ -5233,7 +5230,7 @@
         <v>2</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5577,13 +5574,13 @@
         <v>8001</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C72" s="4">
         <v>2</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>58</v>
@@ -5595,7 +5592,7 @@
         <v>2</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5603,7 +5600,7 @@
         <v>8002</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C73" s="4">
         <v>2</v>
@@ -5621,7 +5618,7 @@
         <v>2</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5629,7 +5626,7 @@
         <v>8003</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C74" s="4">
         <v>2</v>
@@ -5647,7 +5644,7 @@
         <v>2</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5655,7 +5652,7 @@
         <v>8005</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="C75" s="4">
         <v>2</v>
@@ -5673,7 +5670,7 @@
         <v>2</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -10775,7 +10772,7 @@
         <v>0</v>
       </c>
       <c r="D288" s="10" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E288" s="10" t="s">
         <v>59</v>
@@ -10799,7 +10796,7 @@
         <v>0</v>
       </c>
       <c r="D289" s="10" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E289" s="10" t="s">
         <v>59</v>
@@ -10823,7 +10820,7 @@
         <v>0</v>
       </c>
       <c r="D290" s="10" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E290" s="10" t="s">
         <v>59</v>
@@ -10847,7 +10844,7 @@
         <v>0</v>
       </c>
       <c r="D291" s="10" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E291" s="10" t="s">
         <v>59</v>
@@ -10871,7 +10868,7 @@
         <v>0</v>
       </c>
       <c r="D292" s="10" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E292" s="10" t="s">
         <v>59</v>
@@ -10895,7 +10892,7 @@
         <v>0</v>
       </c>
       <c r="D293" s="10" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E293" s="10" t="s">
         <v>59</v>
@@ -10919,7 +10916,7 @@
         <v>0</v>
       </c>
       <c r="D294" s="10" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E294" s="10" t="s">
         <v>59</v>
@@ -10943,7 +10940,7 @@
         <v>0</v>
       </c>
       <c r="D295" s="10" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E295" s="10" t="s">
         <v>59</v>
@@ -10967,7 +10964,7 @@
         <v>0</v>
       </c>
       <c r="D296" s="10" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E296" s="10" t="s">
         <v>159</v>
@@ -10985,13 +10982,13 @@
         <v>8027</v>
       </c>
       <c r="B297" s="10" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C297" s="10">
         <v>0</v>
       </c>
       <c r="D297" s="10" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E297" s="10" t="s">
         <v>752</v>
@@ -11003,7 +11000,7 @@
         <v>6</v>
       </c>
       <c r="H297" s="10" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="298" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -11011,13 +11008,13 @@
         <v>8028</v>
       </c>
       <c r="B298" s="10" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C298" s="10">
         <v>0</v>
       </c>
       <c r="D298" s="10" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="E298" s="10" t="s">
         <v>754</v>
@@ -11029,7 +11026,7 @@
         <v>6</v>
       </c>
       <c r="H298" s="10" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="299" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -11037,13 +11034,13 @@
         <v>8026</v>
       </c>
       <c r="B299" s="10" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C299" s="10">
         <v>0</v>
       </c>
       <c r="D299" s="10" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="E299" s="10" t="s">
         <v>756</v>
@@ -11055,7 +11052,7 @@
         <v>6</v>
       </c>
       <c r="H299" s="10" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="300" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -11063,13 +11060,13 @@
         <v>8163</v>
       </c>
       <c r="B300" s="10" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C300" s="10">
         <v>0</v>
       </c>
       <c r="D300" s="10" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="E300" s="10" t="s">
         <v>493</v>
@@ -11081,7 +11078,7 @@
         <v>6</v>
       </c>
       <c r="H300" s="10" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="301" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -11095,7 +11092,7 @@
         <v>0</v>
       </c>
       <c r="D301" s="10" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="E301" s="10" t="s">
         <v>159</v>
@@ -11119,7 +11116,7 @@
         <v>0</v>
       </c>
       <c r="D302" s="10" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E302" s="10" t="s">
         <v>159</v>
@@ -11143,7 +11140,7 @@
         <v>0</v>
       </c>
       <c r="D303" s="10" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E303" s="10" t="s">
         <v>159</v>
@@ -11161,13 +11158,13 @@
         <v>8042</v>
       </c>
       <c r="B304" s="10" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="C304" s="10">
         <v>0</v>
       </c>
       <c r="D304" s="10" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E304" s="10" t="s">
         <v>762</v>
@@ -11179,7 +11176,7 @@
         <v>6</v>
       </c>
       <c r="H304" s="10" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="305" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -11187,16 +11184,16 @@
         <v>8043</v>
       </c>
       <c r="B305" s="10" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="C305" s="10">
         <v>0</v>
       </c>
       <c r="D305" s="10" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E305" s="10" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="F305" s="10">
         <v>100</v>
@@ -11205,7 +11202,7 @@
         <v>6</v>
       </c>
       <c r="H305" s="10" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="306" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -11213,16 +11210,16 @@
         <v>8014</v>
       </c>
       <c r="B306" s="10" t="s">
+        <v>764</v>
+      </c>
+      <c r="C306" s="10">
+        <v>0</v>
+      </c>
+      <c r="D306" s="10" t="s">
+        <v>832</v>
+      </c>
+      <c r="E306" s="10" t="s">
         <v>765</v>
-      </c>
-      <c r="C306" s="10">
-        <v>0</v>
-      </c>
-      <c r="D306" s="10" t="s">
-        <v>833</v>
-      </c>
-      <c r="E306" s="10" t="s">
-        <v>766</v>
       </c>
       <c r="F306" s="10">
         <v>100</v>
@@ -11231,7 +11228,7 @@
         <v>6</v>
       </c>
       <c r="H306" s="10" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="307" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -11239,16 +11236,16 @@
         <v>8015</v>
       </c>
       <c r="B307" s="10" t="s">
+        <v>766</v>
+      </c>
+      <c r="C307" s="10">
+        <v>0</v>
+      </c>
+      <c r="D307" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="E307" s="10" t="s">
         <v>767</v>
-      </c>
-      <c r="C307" s="10">
-        <v>0</v>
-      </c>
-      <c r="D307" s="10" t="s">
-        <v>834</v>
-      </c>
-      <c r="E307" s="10" t="s">
-        <v>768</v>
       </c>
       <c r="F307" s="10">
         <v>100</v>
@@ -11257,7 +11254,7 @@
         <v>6</v>
       </c>
       <c r="H307" s="10" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="308" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -11265,13 +11262,13 @@
         <v>8016</v>
       </c>
       <c r="B308" s="10" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C308" s="10">
         <v>0</v>
       </c>
       <c r="D308" s="10" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="E308" s="10" t="s">
         <v>762</v>
@@ -11283,7 +11280,7 @@
         <v>6</v>
       </c>
       <c r="H308" s="10" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="309" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -11291,13 +11288,13 @@
         <v>8017</v>
       </c>
       <c r="B309" s="10" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C309" s="10">
         <v>0</v>
       </c>
       <c r="D309" s="10" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E309" s="10" t="s">
         <v>66</v>
@@ -11309,7 +11306,7 @@
         <v>6</v>
       </c>
       <c r="H309" s="10" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="310" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -11317,16 +11314,16 @@
         <v>8021</v>
       </c>
       <c r="B310" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="C310" s="10">
+        <v>0</v>
+      </c>
+      <c r="D310" s="10" t="s">
+        <v>836</v>
+      </c>
+      <c r="E310" s="10" t="s">
         <v>771</v>
-      </c>
-      <c r="C310" s="10">
-        <v>0</v>
-      </c>
-      <c r="D310" s="10" t="s">
-        <v>837</v>
-      </c>
-      <c r="E310" s="10" t="s">
-        <v>772</v>
       </c>
       <c r="F310" s="10">
         <v>100</v>
@@ -11341,16 +11338,16 @@
         <v>8030</v>
       </c>
       <c r="B311" s="10" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C311" s="10">
         <v>0</v>
       </c>
       <c r="D311" s="10" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="E311" s="10" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F311" s="10">
         <v>100</v>
@@ -11365,16 +11362,16 @@
         <v>8040</v>
       </c>
       <c r="B312" s="10" t="s">
+        <v>773</v>
+      </c>
+      <c r="C312" s="10">
+        <v>0</v>
+      </c>
+      <c r="D312" s="10" t="s">
+        <v>838</v>
+      </c>
+      <c r="E312" s="10" t="s">
         <v>774</v>
-      </c>
-      <c r="C312" s="10">
-        <v>0</v>
-      </c>
-      <c r="D312" s="10" t="s">
-        <v>839</v>
-      </c>
-      <c r="E312" s="10" t="s">
-        <v>775</v>
       </c>
       <c r="F312" s="10">
         <v>100</v>
@@ -11389,16 +11386,16 @@
         <v>8047</v>
       </c>
       <c r="B313" s="10" t="s">
+        <v>775</v>
+      </c>
+      <c r="C313" s="10">
+        <v>0</v>
+      </c>
+      <c r="D313" s="10" t="s">
+        <v>839</v>
+      </c>
+      <c r="E313" s="10" t="s">
         <v>776</v>
-      </c>
-      <c r="C313" s="10">
-        <v>0</v>
-      </c>
-      <c r="D313" s="10" t="s">
-        <v>840</v>
-      </c>
-      <c r="E313" s="10" t="s">
-        <v>777</v>
       </c>
       <c r="F313" s="10">
         <v>100</v>
@@ -11413,16 +11410,16 @@
         <v>8099</v>
       </c>
       <c r="B314" s="10" t="s">
+        <v>777</v>
+      </c>
+      <c r="C314" s="10">
+        <v>0</v>
+      </c>
+      <c r="D314" s="10" t="s">
+        <v>840</v>
+      </c>
+      <c r="E314" s="10" t="s">
         <v>778</v>
-      </c>
-      <c r="C314" s="10">
-        <v>0</v>
-      </c>
-      <c r="D314" s="10" t="s">
-        <v>841</v>
-      </c>
-      <c r="E314" s="10" t="s">
-        <v>779</v>
       </c>
       <c r="F314" s="10">
         <v>100</v>
@@ -11437,16 +11434,16 @@
         <v>8079</v>
       </c>
       <c r="B315" s="10" t="s">
+        <v>779</v>
+      </c>
+      <c r="C315" s="10">
+        <v>0</v>
+      </c>
+      <c r="D315" s="10" t="s">
+        <v>841</v>
+      </c>
+      <c r="E315" s="10" t="s">
         <v>780</v>
-      </c>
-      <c r="C315" s="10">
-        <v>0</v>
-      </c>
-      <c r="D315" s="10" t="s">
-        <v>842</v>
-      </c>
-      <c r="E315" s="10" t="s">
-        <v>781</v>
       </c>
       <c r="F315" s="10">
         <v>100</v>
@@ -11461,13 +11458,13 @@
         <v>8080</v>
       </c>
       <c r="B316" s="10" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C316" s="10">
         <v>0</v>
       </c>
       <c r="D316" s="10" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="E316" s="10" t="s">
         <v>262</v>
@@ -11485,16 +11482,16 @@
         <v>8164</v>
       </c>
       <c r="B317" s="10" t="s">
+        <v>782</v>
+      </c>
+      <c r="C317" s="10">
+        <v>0</v>
+      </c>
+      <c r="D317" s="10" t="s">
+        <v>843</v>
+      </c>
+      <c r="E317" s="10" t="s">
         <v>783</v>
-      </c>
-      <c r="C317" s="10">
-        <v>0</v>
-      </c>
-      <c r="D317" s="10" t="s">
-        <v>844</v>
-      </c>
-      <c r="E317" s="10" t="s">
-        <v>784</v>
       </c>
       <c r="F317" s="10">
         <v>100</v>
@@ -11509,16 +11506,16 @@
         <v>8165</v>
       </c>
       <c r="B318" s="10" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C318" s="10">
         <v>0</v>
       </c>
       <c r="D318" s="10" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="E318" s="10" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F318" s="10">
         <v>100</v>
@@ -11527,7 +11524,7 @@
         <v>6</v>
       </c>
       <c r="H318" s="10" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="319" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -11535,16 +11532,16 @@
         <v>8085</v>
       </c>
       <c r="B319" s="10" t="s">
+        <v>785</v>
+      </c>
+      <c r="C319" s="10">
+        <v>0</v>
+      </c>
+      <c r="D319" s="10" t="s">
+        <v>845</v>
+      </c>
+      <c r="E319" s="10" t="s">
         <v>786</v>
-      </c>
-      <c r="C319" s="10">
-        <v>0</v>
-      </c>
-      <c r="D319" s="10" t="s">
-        <v>846</v>
-      </c>
-      <c r="E319" s="10" t="s">
-        <v>787</v>
       </c>
       <c r="F319" s="10">
         <v>100</v>
@@ -11559,16 +11556,16 @@
         <v>8036</v>
       </c>
       <c r="B320" s="10" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C320" s="10">
         <v>0</v>
       </c>
       <c r="D320" s="10" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E320" s="10" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="F320" s="10">
         <v>100</v>
@@ -11583,16 +11580,16 @@
         <v>8034</v>
       </c>
       <c r="B321" s="10" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C321" s="10">
         <v>0</v>
       </c>
       <c r="D321" s="10" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="E321" s="10" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="F321" s="10">
         <v>100</v>
@@ -11607,16 +11604,16 @@
         <v>8035</v>
       </c>
       <c r="B322" s="10" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C322" s="10">
         <v>0</v>
       </c>
       <c r="D322" s="10" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="E322" s="10" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F322" s="10">
         <v>100</v>
@@ -11631,16 +11628,16 @@
         <v>8095</v>
       </c>
       <c r="B323" s="10" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C323" s="10">
         <v>0</v>
       </c>
       <c r="D323" s="10" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="E323" s="10" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F323" s="10">
         <v>100</v>
@@ -11655,16 +11652,16 @@
         <v>8094</v>
       </c>
       <c r="B324" s="10" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C324" s="10">
         <v>0</v>
       </c>
       <c r="D324" s="10" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E324" s="10" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="F324" s="10">
         <v>100</v>
@@ -11679,13 +11676,13 @@
         <v>8031</v>
       </c>
       <c r="B325" s="10" t="s">
+        <v>869</v>
+      </c>
+      <c r="C325" s="10">
+        <v>0</v>
+      </c>
+      <c r="D325" s="10" t="s">
         <v>870</v>
-      </c>
-      <c r="C325" s="10">
-        <v>0</v>
-      </c>
-      <c r="D325" s="10" t="s">
-        <v>871</v>
       </c>
       <c r="E325" s="10" t="s">
         <v>64</v>
@@ -11697,7 +11694,7 @@
         <v>6</v>
       </c>
       <c r="H325" s="10" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="326" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -11705,16 +11702,16 @@
         <v>8011</v>
       </c>
       <c r="B326" s="10" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C326" s="10">
         <v>0</v>
       </c>
       <c r="D326" s="10" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E326" s="10" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="F326" s="10">
         <v>100</v>
@@ -11729,16 +11726,16 @@
         <v>8166</v>
       </c>
       <c r="B327" s="10" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C327" s="10">
         <v>0</v>
       </c>
       <c r="D327" s="10" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E327" s="10" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F327" s="10">
         <v>100</v>
@@ -11747,7 +11744,7 @@
         <v>6</v>
       </c>
       <c r="H327" s="10" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="328" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -11755,16 +11752,16 @@
         <v>8172</v>
       </c>
       <c r="B328" s="10" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C328" s="10">
         <v>0</v>
       </c>
       <c r="D328" s="10" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E328" s="10" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="F328" s="10">
         <v>100</v>
@@ -11779,16 +11776,16 @@
         <v>8167</v>
       </c>
       <c r="B329" s="10" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C329" s="10">
         <v>0</v>
       </c>
       <c r="D329" s="10" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E329" s="10" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F329" s="10">
         <v>100</v>
@@ -11803,16 +11800,16 @@
         <v>8168</v>
       </c>
       <c r="B330" s="10" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C330" s="10">
         <v>0</v>
       </c>
       <c r="D330" s="10" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="E330" s="10" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="F330" s="10">
         <v>100</v>
@@ -11827,16 +11824,16 @@
         <v>8169</v>
       </c>
       <c r="B331" s="10" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C331" s="10">
         <v>0</v>
       </c>
       <c r="D331" s="10" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="E331" s="10" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="F331" s="10">
         <v>100</v>
@@ -11851,16 +11848,16 @@
         <v>8170</v>
       </c>
       <c r="B332" s="10" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C332" s="10">
         <v>0</v>
       </c>
       <c r="D332" s="10" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="E332" s="10" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="F332" s="10">
         <v>100</v>
@@ -11875,16 +11872,16 @@
         <v>8200</v>
       </c>
       <c r="B333" s="10" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C333" s="10">
         <v>0</v>
       </c>
       <c r="D333" s="10" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="E333" s="10" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F333" s="10">
         <v>100</v>
@@ -11899,16 +11896,16 @@
         <v>8201</v>
       </c>
       <c r="B334" s="10" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C334" s="10">
         <v>0</v>
       </c>
       <c r="D334" s="10" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="E334" s="10" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F334" s="10">
         <v>100</v>
@@ -11923,16 +11920,16 @@
         <v>8202</v>
       </c>
       <c r="B335" s="10" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C335" s="10">
         <v>0</v>
       </c>
       <c r="D335" s="10" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="E335" s="10" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F335" s="10">
         <v>100</v>
@@ -11947,16 +11944,16 @@
         <v>8203</v>
       </c>
       <c r="B336" s="10" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C336" s="10">
         <v>0</v>
       </c>
       <c r="D336" s="10" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="E336" s="10" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F336" s="10">
         <v>100</v>
@@ -11971,16 +11968,16 @@
         <v>8072</v>
       </c>
       <c r="B337" s="10" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C337" s="10">
         <v>0</v>
       </c>
       <c r="D337" s="10" t="s">
+        <v>862</v>
+      </c>
+      <c r="E337" s="10" t="s">
         <v>863</v>
-      </c>
-      <c r="E337" s="10" t="s">
-        <v>864</v>
       </c>
       <c r="F337" s="10">
         <v>6000</v>
@@ -12002,7 +11999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:N1048576"/>
     </sheetView>
   </sheetViews>
@@ -19080,8 +19077,8 @@
   <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -19271,7 +19268,7 @@
         <v>8043</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>763</v>
+        <v>886</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -19279,7 +19276,7 @@
         <v>8014</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -19287,7 +19284,7 @@
         <v>8015</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -19295,7 +19292,7 @@
         <v>8016</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -19303,7 +19300,7 @@
         <v>8017</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -19311,7 +19308,7 @@
         <v>8021</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -19319,7 +19316,7 @@
         <v>8030</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -19327,7 +19324,7 @@
         <v>8040</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -19335,7 +19332,7 @@
         <v>8047</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -19343,7 +19340,7 @@
         <v>8099</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -19351,7 +19348,7 @@
         <v>8079</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -19359,7 +19356,7 @@
         <v>8080</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -19367,7 +19364,7 @@
         <v>8164</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -19375,7 +19372,7 @@
         <v>8165</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -19383,7 +19380,7 @@
         <v>8085</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -19391,7 +19388,7 @@
         <v>8036</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -19399,7 +19396,7 @@
         <v>8034</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -19407,7 +19404,7 @@
         <v>8035</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -19415,7 +19412,7 @@
         <v>8095</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -19423,7 +19420,7 @@
         <v>8094</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -19431,7 +19428,7 @@
         <v>8031</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -19439,7 +19436,7 @@
         <v>8011</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -19447,7 +19444,7 @@
         <v>8166</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -19455,7 +19452,7 @@
         <v>8172</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -19463,7 +19460,7 @@
         <v>8167</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -19471,7 +19468,7 @@
         <v>8168</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -19479,7 +19476,7 @@
         <v>8169</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -19487,7 +19484,7 @@
         <v>8170</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -19495,7 +19492,7 @@
         <v>8200</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -19503,7 +19500,7 @@
         <v>8201</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -19511,7 +19508,7 @@
         <v>8202</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -19519,7 +19516,7 @@
         <v>8203</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -19527,7 +19524,7 @@
         <v>8072</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="56" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add Some Quest for JuLu
</commit_message>
<xml_diff>
--- a/Excels/SchemaItems.xlsx
+++ b/Excels/SchemaItems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\GitHub\TKSR\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17C5874-6E35-4F96-B3ED-7CB59846A31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B5D8E9-CFC6-4525-BFB3-DCF7E1DB3A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="914">
   <si>
     <t>Id</t>
   </si>
@@ -3301,6 +3301,30 @@
   </si>
   <si>
     <t>QuestPropCnt_HuRou</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestPropCnt_QingXiang</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestPropCnt_HaiLuo</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestPropCnt_HuangFuZhi</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄符纸</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>海螺</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>清香</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -3828,8 +3852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2BF42B-B9E6-4AA7-A0C5-A2602055F321}">
   <dimension ref="A1:H337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
-      <selection activeCell="H305" sqref="H305"/>
+    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
+      <selection activeCell="B320" sqref="B320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -11556,7 +11580,7 @@
         <v>8036</v>
       </c>
       <c r="B320" s="10" t="s">
-        <v>787</v>
+        <v>913</v>
       </c>
       <c r="C320" s="10">
         <v>0</v>
@@ -11573,14 +11597,16 @@
       <c r="G320" s="10">
         <v>6</v>
       </c>
-      <c r="H320" s="10"/>
+      <c r="H320" s="10" t="s">
+        <v>908</v>
+      </c>
     </row>
     <row r="321" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A321" s="10">
         <v>8034</v>
       </c>
       <c r="B321" s="10" t="s">
-        <v>788</v>
+        <v>912</v>
       </c>
       <c r="C321" s="10">
         <v>0</v>
@@ -11597,14 +11623,16 @@
       <c r="G321" s="10">
         <v>6</v>
       </c>
-      <c r="H321" s="10"/>
+      <c r="H321" s="10" t="s">
+        <v>909</v>
+      </c>
     </row>
     <row r="322" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A322" s="10">
         <v>8035</v>
       </c>
       <c r="B322" s="10" t="s">
-        <v>790</v>
+        <v>911</v>
       </c>
       <c r="C322" s="10">
         <v>0</v>
@@ -11621,7 +11649,9 @@
       <c r="G322" s="10">
         <v>6</v>
       </c>
-      <c r="H322" s="10"/>
+      <c r="H322" s="10" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="323" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A323" s="10">

</xml_diff>

<commit_message>
Add Some Assets for XieLiang GuanYu Quest
</commit_message>
<xml_diff>
--- a/Excels/SchemaItems.xlsx
+++ b/Excels/SchemaItems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\GitHub\TKSR\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B5D8E9-CFC6-4525-BFB3-DCF7E1DB3A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6C4745-4089-4BF0-8ED9-E6FE4F0AD50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="914">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="922">
   <si>
     <t>Id</t>
   </si>
@@ -3325,6 +3325,38 @@
   </si>
   <si>
     <t>清香</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestPropCnt_WenWangGuaQian</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestPropCnt_LingPai</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestPropCnt_ShanShuPi</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestPropCnt_GanTai</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestPropCnt_CaiQiu</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestPropCnt_CaiDai</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestPropCnt_LingGu</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestPropCnt_FengChe</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -3852,8 +3884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2BF42B-B9E6-4AA7-A0C5-A2602055F321}">
   <dimension ref="A1:H337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="B320" sqref="B320"/>
+    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
+      <selection activeCell="H313" sqref="H313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -11427,7 +11459,9 @@
       <c r="G313" s="10">
         <v>6</v>
       </c>
-      <c r="H313" s="10"/>
+      <c r="H313" s="10" t="s">
+        <v>915</v>
+      </c>
     </row>
     <row r="314" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A314" s="10">
@@ -11451,7 +11485,9 @@
       <c r="G314" s="10">
         <v>6</v>
       </c>
-      <c r="H314" s="10"/>
+      <c r="H314" s="10" t="s">
+        <v>914</v>
+      </c>
     </row>
     <row r="315" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A315" s="10">
@@ -11675,7 +11711,9 @@
       <c r="G323" s="10">
         <v>6</v>
       </c>
-      <c r="H323" s="10"/>
+      <c r="H323" s="10" t="s">
+        <v>917</v>
+      </c>
     </row>
     <row r="324" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A324" s="10">
@@ -11699,7 +11737,9 @@
       <c r="G324" s="10">
         <v>6</v>
       </c>
-      <c r="H324" s="10"/>
+      <c r="H324" s="10" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="325" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A325" s="10">
@@ -11823,7 +11863,9 @@
       <c r="G329" s="10">
         <v>6</v>
       </c>
-      <c r="H329" s="10"/>
+      <c r="H329" s="10" t="s">
+        <v>918</v>
+      </c>
     </row>
     <row r="330" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A330" s="10">
@@ -11847,7 +11889,9 @@
       <c r="G330" s="10">
         <v>6</v>
       </c>
-      <c r="H330" s="10"/>
+      <c r="H330" s="10" t="s">
+        <v>919</v>
+      </c>
     </row>
     <row r="331" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A331" s="10">
@@ -11871,7 +11915,9 @@
       <c r="G331" s="10">
         <v>6</v>
       </c>
-      <c r="H331" s="10"/>
+      <c r="H331" s="10" t="s">
+        <v>920</v>
+      </c>
     </row>
     <row r="332" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A332" s="10">
@@ -11895,7 +11941,9 @@
       <c r="G332" s="10">
         <v>6</v>
       </c>
-      <c r="H332" s="10"/>
+      <c r="H332" s="10" t="s">
+        <v>921</v>
+      </c>
     </row>
     <row r="333" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A333" s="10">

</xml_diff>